<commit_message>
new component to upload, url not yet saved
</commit_message>
<xml_diff>
--- a/test_file.xlsx
+++ b/test_file.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/esme-marie/Desktop/RebootFSDB/FullStackProject/myschooladmin/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/esme-marie/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E745539F-36EC-694C-9E1D-65FC419C336A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B0C59CBD-CCEF-004A-8BC8-B18581BF5559}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6120" yWindow="460" windowWidth="13200" windowHeight="14900" xr2:uid="{68CB82FE-8313-5849-BC9F-818D344539F1}"/>
+    <workbookView xWindow="680" yWindow="960" windowWidth="26340" windowHeight="13920" xr2:uid="{3F2FA6ED-DF49-E24C-8249-159581959265}"/>
   </bookViews>
   <sheets>
     <sheet name="grades" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="26">
   <si>
     <t>subject_id</t>
   </si>
@@ -39,28 +39,70 @@
     <t>semester_assessment</t>
   </si>
   <si>
+    <t>LAM01</t>
+  </si>
+  <si>
+    <t>FTM001</t>
+  </si>
+  <si>
     <t>Mid-Sem_1/2020-2021</t>
   </si>
   <si>
-    <t>FSD02</t>
-  </si>
-  <si>
-    <t>RBT001</t>
-  </si>
-  <si>
-    <t>RBT002</t>
-  </si>
-  <si>
-    <t>RBT003</t>
-  </si>
-  <si>
-    <t>RBT004</t>
-  </si>
-  <si>
-    <t>RBT005</t>
-  </si>
-  <si>
-    <t>RBT006</t>
+    <t>FTJ001</t>
+  </si>
+  <si>
+    <t>FTU001</t>
+  </si>
+  <si>
+    <t>FTS002</t>
+  </si>
+  <si>
+    <t>LAU01</t>
+  </si>
+  <si>
+    <t>FTM002</t>
+  </si>
+  <si>
+    <t>FTK001</t>
+  </si>
+  <si>
+    <t>FTB001</t>
+  </si>
+  <si>
+    <t>FTJ002</t>
+  </si>
+  <si>
+    <t>FTJ003</t>
+  </si>
+  <si>
+    <t>FTS001</t>
+  </si>
+  <si>
+    <t>FTU002</t>
+  </si>
+  <si>
+    <t>MYL02</t>
+  </si>
+  <si>
+    <t>MSM03</t>
+  </si>
+  <si>
+    <t>MSU03</t>
+  </si>
+  <si>
+    <t>SEM04</t>
+  </si>
+  <si>
+    <t>SEU04</t>
+  </si>
+  <si>
+    <t>HYM05</t>
+  </si>
+  <si>
+    <t>HYU05</t>
+  </si>
+  <si>
+    <t>WRG06</t>
   </si>
 </sst>
 </file>
@@ -76,7 +118,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -105,10 +148,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -119,12 +163,16 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Per cent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -435,11 +483,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC8F689B-83CF-9B47-AC66-5E36C5BC99BD}">
-  <dimension ref="A1:D7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C01B0A6-AD66-6847-94BB-FD5EB445CBE1}">
+  <dimension ref="A1:D67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="99" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -464,91 +512,930 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="C2" s="3">
-        <v>94</v>
+        <v>92.5</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="3">
-        <v>95</v>
+        <v>74.5</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
-        <v>5</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="3">
-        <v>96</v>
+      <c r="C4" s="4">
+        <v>89</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
-        <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="3">
+        <v>78</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="3">
+        <v>85.5</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="3">
+        <v>98</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="3">
+        <v>88</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="3">
+        <v>78.5</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="3">
+        <v>72</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="3">
+        <v>98</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="3">
+        <v>75.5</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="3">
+        <v>88</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="3">
+        <v>66</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="4">
+        <v>94</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="3">
+        <v>65</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="3">
+        <v>82</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="3">
+        <v>92</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="3">
+        <v>82</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="3">
+        <v>62</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="3">
+        <v>55</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" s="3">
+        <v>92</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="3">
+        <v>90</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="3">
+        <v>80</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="3">
+        <v>82</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" s="3">
+        <v>85</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" s="3">
+        <v>82</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" s="3">
+        <v>78</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29" s="3">
+        <v>95</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="3">
+        <v>84.5</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" s="3">
+        <v>79</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C32" s="3">
+        <v>75.5</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C33" s="3">
+        <v>90</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C34" s="3">
+        <v>69</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" s="3">
+        <v>75.5</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36" s="3">
+        <v>83.5</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37" s="3">
+        <v>88.5</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C38" s="3">
+        <v>80.5</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C39" s="3">
+        <v>85.5</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C40" s="3">
+        <v>97.5</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C41" s="3">
+        <v>93.5</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C42" s="3">
+        <v>83.5</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C43" s="3">
+        <v>79.5</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C44" s="3">
+        <v>98.5</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C45" s="3">
+        <v>82</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C46" s="3">
+        <v>95.5</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C47" s="3">
+        <v>74.5</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C48" s="3">
+        <v>88</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C49" s="3">
+        <v>78</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C50" s="3">
         <v>97</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+      <c r="D50" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C51" s="3">
+        <v>93</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C52" s="3">
+        <v>98</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C53" s="3">
+        <v>68</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C54" s="3">
+        <v>59</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C55" s="3">
+        <v>96.5</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C56" s="3">
+        <v>76</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B57" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="3">
-        <v>98</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="2" t="s">
+      <c r="C57" s="3">
+        <v>96</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C58" s="3">
+        <v>58.5</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C59" s="3">
+        <v>85.5</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C60" s="3">
+        <v>65</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B61" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="3">
-        <v>99</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>4</v>
+      <c r="C61" s="3">
+        <v>93</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C62" s="3">
+        <v>95.5</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C63" s="3">
+        <v>92.5</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C64" s="3">
+        <v>55.5</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C65" s="3">
+        <v>53</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C66" s="3">
+        <v>98.5</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C67" s="3">
+        <v>79</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>